<commit_message>
update code redirection page and list
</commit_message>
<xml_diff>
--- a/JDT/JDT_AlessioLopardo.xlsx
+++ b/JDT/JDT_AlessioLopardo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu41ecx\Documents\GitHub\P-AppMobile\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B9C5A-505A-4012-B18E-07D34C0571F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6377984D-A2A6-40ED-9596-3AA36CBAFCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t xml:space="preserve">Code de la page tableau de bord </t>
+  </si>
+  <si>
+    <t>Rajout des icons sur la maquette pour la bar menu</t>
+  </si>
+  <si>
+    <t>Recherche fonctionnalité de redirection sur une autre page lors de la sélection d'un bouton / image.</t>
+  </si>
+  <si>
+    <t>Recherche fonctionnalité de model / template pour l'affichage des livres.</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1075,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2083333333333336E-2</c:v>
+                  <c:v>0.1388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1081,7 +1090,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1997,7 +2006,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2050,7 +2059,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 5 heurs 0 minutes</v>
+        <v>0 jours 7 heurs 15 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2065,15 +2074,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>300</v>
+        <v>435</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2277,15 +2286,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="str">
+      <c r="A13" s="17">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="51"/>
+        <v>16</v>
+      </c>
+      <c r="B13" s="51">
+        <v>45397</v>
+      </c>
       <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="53">
+        <v>10</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="18"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2297,16 +2314,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+    <row r="14" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="47">
+        <v>45397</v>
+      </c>
+      <c r="C14" s="48">
+        <v>1</v>
+      </c>
       <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2319,15 +2344,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="str">
+      <c r="A15" s="17">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="37"/>
+        <v>16</v>
+      </c>
+      <c r="B15" s="51">
+        <v>45397</v>
+      </c>
+      <c r="C15" s="52">
+        <v>1</v>
+      </c>
+      <c r="D15" s="53">
+        <v>5</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -8658,11 +8693,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8670,7 +8705,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>5.2083333333333336E-2</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8748,7 +8783,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C10" s="38" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8756,7 +8791,7 @@
       </c>
       <c r="D10" s="34">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8779,7 +8814,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.125</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8802,17 +8837,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9035,6 +9059,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9044,17 +9079,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9071,4 +9095,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
formating and stylising book list
</commit_message>
<xml_diff>
--- a/JDT/JDT_AlessioLopardo.xlsx
+++ b/JDT/JDT_AlessioLopardo.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu41ecx\Documents\GitHub\P-AppMobile\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6377984D-A2A6-40ED-9596-3AA36CBAFCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D808043F-452D-4FCD-9857-1D2BA54269BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="840" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>Recherche fonctionnalité de model / template pour l'affichage des livres.</t>
+  </si>
+  <si>
+    <t>Mise en place du menu tab en bas de l'écran pour naviguer entre la liste de livre et le livre en lecture.</t>
+  </si>
+  <si>
+    <t>Factorisation de la mise en forme de la page de liste. Création de la grid pour la mise en page et disposition des livre. Petits problème pour afficher les livre, en changer la source de celle local a celle sur internet les livres s'affichaient. Pour le bord des livre problème avec la balise "border" car elle n'accepte qu'un seul élément, la balise "frame" et plus efficace.</t>
+  </si>
+  <si>
+    <t>Recherche et mise en place d'une palette de couleur.</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1084,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1388888888888889</c:v>
+                  <c:v>0.2326388888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2005,8 +2014,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2068,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 15 minutes</v>
+        <v>0 jours 9 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2074,15 +2083,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>195</v>
+        <v>270</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>435</v>
+        <v>570</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2374,31 +2383,49 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+    <row r="16" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="47">
+        <v>45404</v>
+      </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="37"/>
+      <c r="D16" s="49">
+        <v>10</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="16"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="str">
+    <row r="17" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="37"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="51">
+        <v>45404</v>
+      </c>
+      <c r="C17" s="52">
+        <v>1</v>
+      </c>
+      <c r="D17" s="53">
+        <v>35</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="O17">
         <v>45</v>
@@ -2411,9 +2438,15 @@
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="37"/>
+      <c r="D18" s="49">
+        <v>30</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="16"/>
       <c r="O18">
         <v>50</v>
@@ -8693,11 +8726,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8705,7 +8738,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.1388888888888889</v>
+        <v>0.2326388888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8814,7 +8847,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.21875</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8837,6 +8870,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9059,17 +9103,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9079,6 +9112,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9095,15 +9139,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
try to read epub file
</commit_message>
<xml_diff>
--- a/JDT/JDT_AlessioLopardo.xlsx
+++ b/JDT/JDT_AlessioLopardo.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu41ecx\Documents\GitHub\P-AppMobile\JDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu41ecx\Documents\GitHub\P-335-ReadMe\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D808043F-452D-4FCD-9857-1D2BA54269BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33B022C-DAD8-4944-AE7C-0CEFEEA5E3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Recherche et mise en place d'une palette de couleur.</t>
+  </si>
+  <si>
+    <t>Intégration du MVVM dans le projet, abandon car pour la suite trop compliquer en sachant que nous venons de commencer le model MVVM</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1087,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2326388888888889</c:v>
+                  <c:v>0.2638888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2068,7 +2071,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 30 minutes</v>
+        <v>0 jours 10 heurs 15 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2087,11 +2090,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>570</v>
+        <v>615</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2432,11 +2435,13 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="47">
+        <v>45404</v>
+      </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49">
         <v>30</v>
@@ -2452,16 +2457,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="str">
+    <row r="19" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="51">
+        <v>45411</v>
+      </c>
       <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="37"/>
+      <c r="D19" s="53">
+        <v>45</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="18"/>
       <c r="O19">
         <v>55</v>
@@ -8730,7 +8743,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8738,7 +8751,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.2326388888888889</v>
+        <v>0.2638888888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8847,7 +8860,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.3125</v>
+        <v>0.34375</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8870,17 +8883,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9103,6 +9105,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9112,17 +9125,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9139,4 +9141,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>